<commit_message>
Screenshots for GW 19
</commit_message>
<xml_diff>
--- a/EPLPredictorBackend/PLResults.xlsx
+++ b/EPLPredictorBackend/PLResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saahil Parikh\Projects\EPLPredictor\EPLPredictorBackend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4968C81-8250-4F55-B2B5-0230A21E6486}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CAFB01-D9AC-40FB-86EE-00F01CD64D0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="366">
   <si>
     <t>Home Team</t>
   </si>
@@ -1092,6 +1092,42 @@
   </si>
   <si>
     <t>1.37204</t>
+  </si>
+  <si>
+    <t>2.01315</t>
+  </si>
+  <si>
+    <t>1.04745</t>
+  </si>
+  <si>
+    <t>0.852495</t>
+  </si>
+  <si>
+    <t>0.323445</t>
+  </si>
+  <si>
+    <t>0.648582</t>
+  </si>
+  <si>
+    <t>1.23996</t>
+  </si>
+  <si>
+    <t>2.90855</t>
+  </si>
+  <si>
+    <t>0.177084</t>
+  </si>
+  <si>
+    <t>3.14372</t>
+  </si>
+  <si>
+    <t>1.05329</t>
+  </si>
+  <si>
+    <t>0.368554</t>
+  </si>
+  <si>
+    <t>0.709634</t>
   </si>
 </sst>
 </file>
@@ -1431,10 +1467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F165"/>
+  <dimension ref="A1:F171"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="E166" sqref="E166"/>
+      <selection activeCell="E172" sqref="E172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4172,7 +4208,7 @@
         <v>48.3</v>
       </c>
       <c r="F130">
-        <f t="shared" ref="F130:F193" si="4">SUM(100-E130)</f>
+        <f t="shared" ref="F130:F161" si="4">SUM(100-E130)</f>
         <v>51.7</v>
       </c>
     </row>
@@ -4844,7 +4880,7 @@
         <v>38.1</v>
       </c>
       <c r="F162">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="F162:F193" si="5">SUM(100-E162)</f>
         <v>61.9</v>
       </c>
     </row>
@@ -4865,7 +4901,7 @@
         <v>43.3</v>
       </c>
       <c r="F163">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>56.7</v>
       </c>
     </row>
@@ -4886,7 +4922,7 @@
         <v>54.6</v>
       </c>
       <c r="F164">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>45.4</v>
       </c>
     </row>
@@ -4907,8 +4943,134 @@
         <v>33</v>
       </c>
       <c r="F165">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>67</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>30</v>
+      </c>
+      <c r="B166" t="s">
+        <v>19</v>
+      </c>
+      <c r="C166" t="s">
+        <v>354</v>
+      </c>
+      <c r="D166" t="s">
+        <v>355</v>
+      </c>
+      <c r="E166">
+        <v>66.2</v>
+      </c>
+      <c r="F166">
+        <f t="shared" si="5"/>
+        <v>33.799999999999997</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>31</v>
+      </c>
+      <c r="B167" t="s">
+        <v>27</v>
+      </c>
+      <c r="C167" t="s">
+        <v>356</v>
+      </c>
+      <c r="D167" t="s">
+        <v>357</v>
+      </c>
+      <c r="E167">
+        <v>52.8</v>
+      </c>
+      <c r="F167">
+        <f t="shared" si="5"/>
+        <v>47.2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>53</v>
+      </c>
+      <c r="B168" t="s">
+        <v>42</v>
+      </c>
+      <c r="C168" t="s">
+        <v>358</v>
+      </c>
+      <c r="D168" t="s">
+        <v>359</v>
+      </c>
+      <c r="E168">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="F168">
+        <f t="shared" si="5"/>
+        <v>62.7</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>59</v>
+      </c>
+      <c r="B169" t="s">
+        <v>34</v>
+      </c>
+      <c r="C169" t="s">
+        <v>360</v>
+      </c>
+      <c r="D169" t="s">
+        <v>361</v>
+      </c>
+      <c r="E169">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="F169">
+        <f t="shared" si="5"/>
+        <v>34.900000000000006</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>26</v>
+      </c>
+      <c r="B170" t="s">
+        <v>6</v>
+      </c>
+      <c r="C170" t="s">
+        <v>362</v>
+      </c>
+      <c r="D170" t="s">
+        <v>363</v>
+      </c>
+      <c r="E170">
+        <v>52.4</v>
+      </c>
+      <c r="F170">
+        <f t="shared" si="5"/>
+        <v>47.6</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>7</v>
+      </c>
+      <c r="B171" t="s">
+        <v>10</v>
+      </c>
+      <c r="C171" t="s">
+        <v>364</v>
+      </c>
+      <c r="D171" t="s">
+        <v>365</v>
+      </c>
+      <c r="E171">
+        <v>67.2</v>
+      </c>
+      <c r="F171">
+        <f t="shared" si="5"/>
+        <v>32.799999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>